<commit_message>
SSABoosterSup: Update spreadsheet. Alarm settings using DOL and OUT from ao record
</commit_message>
<xml_diff>
--- a/documentation/SSABooster/Variáveis Aquisição Booster.xlsx
+++ b/documentation/SSABooster/Variáveis Aquisição Booster.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21805"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21811"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\david.daminelli@lnls.br\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{47ACE303-FA64-422A-A1DF-B4F36CF2F27D}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{B45ECC22-C1FD-4ACD-B305-CB2C5A093A08}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="5025" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -18900,12 +18900,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
 </p:properties>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x0101001FADEDC2238D1B459B3876E2C2E99497" ma:contentTypeVersion="8" ma:contentTypeDescription="Crie um novo documento." ma:contentTypeScope="" ma:versionID="e2216931ecfa3ed1671143eb7091a50c">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="40443515-7982-453e-8cc3-61a478897d4d" xmlns:ns3="32dc2326-b69f-4ff3-bc41-ce299fdac243" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="9c4ad10e40a35dea085704c72c01ed87" ns2:_="" ns3:_="">
     <xsd:import namespace="40443515-7982-453e-8cc3-61a478897d4d"/>
@@ -19096,23 +19105,14 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A45D103D-A57F-47D5-B272-EC4090B47FD6}"/>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{210FDAB5-8E17-4762-B1CB-54C1272C90BC}"/>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6A910CF9-51B6-440E-AF9A-CF1ACA615005}"/>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A45D103D-A57F-47D5-B272-EC4090B47FD6}"/>
 </file>
</xml_diff>